<commit_message>
adding menu to main prj
</commit_message>
<xml_diff>
--- a/Iran-Pop.xlsx
+++ b/Iran-Pop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MT1ShotYT\Desktop\Music-Categorizer\Music-Categorizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E002AA3-AF7B-4853-9728-7D79C1F707CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C0BC6B-3A2B-4F0E-9C51-BCBBAC24BC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>Names</t>
   </si>
@@ -314,6 +314,15 @@
   </si>
   <si>
     <t>Jafar</t>
+  </si>
+  <si>
+    <t>TM Bax</t>
+  </si>
+  <si>
+    <t>Tm Bax</t>
+  </si>
+  <si>
+    <t>TM BAX</t>
   </si>
 </sst>
 </file>
@@ -653,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A101"/>
+  <dimension ref="A1:A104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,6 +1178,21 @@
         <v>97</v>
       </c>
     </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding country & fix a small bug
</commit_message>
<xml_diff>
--- a/Iran-Pop.xlsx
+++ b/Iran-Pop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MT1ShotYT\Desktop\Music-Categorizer\Music-Categorizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84D856B-E789-4C36-99DB-C9853D02A067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A84E3C7-B704-41C7-B652-5F00F2E96F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="16320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
   <si>
     <t>Names</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>Tohi</t>
+  </si>
+  <si>
+    <t>Mohamad Alizadeh</t>
   </si>
 </sst>
 </file>
@@ -671,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A107"/>
+  <dimension ref="A1:A108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
       <selection activeCell="A108" sqref="A108"/>
@@ -1217,6 +1220,11 @@
         <v>103</v>
       </c>
     </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lower case for name checking
</commit_message>
<xml_diff>
--- a/Iran-Pop.xlsx
+++ b/Iran-Pop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MT1ShotYT\Desktop\Music-Categorizer\Music-Categorizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A84E3C7-B704-41C7-B652-5F00F2E96F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69119BD-7ABB-4201-8366-AAE12AC0E0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="16320" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="111">
   <si>
     <t>Names</t>
   </si>
@@ -335,6 +335,24 @@
   </si>
   <si>
     <t>Mohamad Alizadeh</t>
+  </si>
+  <si>
+    <t>Shahin Loo</t>
+  </si>
+  <si>
+    <t>Talk down</t>
+  </si>
+  <si>
+    <t>Armin 2afm</t>
+  </si>
+  <si>
+    <t>armin 2afm</t>
+  </si>
+  <si>
+    <t>Armin zarei</t>
+  </si>
+  <si>
+    <t>Armin Zarei</t>
   </si>
 </sst>
 </file>
@@ -674,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A108"/>
+  <dimension ref="A1:A116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,6 +1243,46 @@
         <v>104</v>
       </c>
     </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>